<commit_message>
Not sure how to handle empty plots that have cover values, but have handled Not_Seeded_Cover col
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/04.2b_edited-species-seeded1_SpeciesSeeded-in-mix-assigned.xlsx
+++ b/data/data-wrangling-intermediate/04.2b_edited-species-seeded1_SpeciesSeeded-in-mix-assigned.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="266" documentId="13_ncr:40009_{4E2DAE92-AEF9-46BE-997C-3D03E1D04585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70FEAA75-BEEA-4F2C-B6CD-4A1FD9DB0E6A}"/>
+  <xr:revisionPtr revIDLastSave="287" documentId="13_ncr:40009_{4E2DAE92-AEF9-46BE-997C-3D03E1D04585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B8A31D8-366A-4558-9B84-6FEB686DDEC6}"/>
   <bookViews>
-    <workbookView xWindow="41295" yWindow="0" windowWidth="12810" windowHeight="15135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1974" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2044" uniqueCount="247">
   <si>
     <t>Region</t>
   </si>
@@ -755,6 +755,12 @@
   </si>
   <si>
     <t>Encelia farinosa</t>
+  </si>
+  <si>
+    <t>AMDE4</t>
+  </si>
+  <si>
+    <t>Ambrosia deltoidea</t>
   </si>
 </sst>
 </file>
@@ -1809,11 +1815,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G282"/>
+  <dimension ref="A1:G292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26:D26"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3398,16 +3404,16 @@
         <v>67</v>
       </c>
       <c r="C69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D69" t="s">
-        <v>68</v>
+        <v>245</v>
       </c>
       <c r="E69" t="s">
-        <v>68</v>
+        <v>245</v>
       </c>
       <c r="F69" t="s">
-        <v>194</v>
+        <v>246</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>161</v>
@@ -3418,22 +3424,22 @@
         <v>66</v>
       </c>
       <c r="B70" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C70" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D70" t="s">
-        <v>72</v>
+        <v>243</v>
       </c>
       <c r="E70" t="s">
-        <v>72</v>
+        <v>243</v>
       </c>
       <c r="F70" t="s">
-        <v>196</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>161</v>
+        <v>244</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -3441,19 +3447,19 @@
         <v>66</v>
       </c>
       <c r="B71" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C71" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D71" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="E71" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="F71" t="s">
-        <v>166</v>
+        <v>194</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>161</v>
@@ -3464,22 +3470,22 @@
         <v>66</v>
       </c>
       <c r="B72" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C72" t="s">
         <v>21</v>
       </c>
       <c r="D72" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="E72" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="F72" t="s">
-        <v>164</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>201</v>
+        <v>182</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -3487,19 +3493,19 @@
         <v>66</v>
       </c>
       <c r="B73" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C73" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D73" t="s">
-        <v>243</v>
+        <v>69</v>
       </c>
       <c r="E73" t="s">
-        <v>243</v>
+        <v>70</v>
       </c>
       <c r="F73" t="s">
-        <v>244</v>
+        <v>195</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>201</v>
@@ -3510,22 +3516,22 @@
         <v>66</v>
       </c>
       <c r="B74" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C74" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D74" t="s">
-        <v>74</v>
+        <v>245</v>
       </c>
       <c r="E74" t="s">
-        <v>74</v>
+        <v>245</v>
       </c>
       <c r="F74" t="s">
-        <v>197</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>161</v>
+        <v>246</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -3533,19 +3539,19 @@
         <v>66</v>
       </c>
       <c r="B75" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C75" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D75" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="E75" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="F75" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>161</v>
@@ -3556,19 +3562,19 @@
         <v>66</v>
       </c>
       <c r="B76" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C76" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D76" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E76" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F76" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>161</v>
@@ -3579,22 +3585,22 @@
         <v>66</v>
       </c>
       <c r="B77" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C77" t="s">
         <v>9</v>
       </c>
       <c r="D77" t="s">
-        <v>243</v>
+        <v>74</v>
       </c>
       <c r="E77" t="s">
-        <v>243</v>
+        <v>74</v>
       </c>
       <c r="F77" t="s">
-        <v>244</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -3602,19 +3608,19 @@
         <v>66</v>
       </c>
       <c r="B78" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C78" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D78" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="E78" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="F78" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>201</v>
@@ -3625,19 +3631,19 @@
         <v>66</v>
       </c>
       <c r="B79" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C79" t="s">
         <v>21</v>
       </c>
       <c r="D79" t="s">
-        <v>69</v>
+        <v>245</v>
       </c>
       <c r="E79" t="s">
-        <v>70</v>
+        <v>245</v>
       </c>
       <c r="F79" t="s">
-        <v>195</v>
+        <v>246</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>201</v>
@@ -3648,180 +3654,180 @@
         <v>66</v>
       </c>
       <c r="B80" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C80" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D80" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="E80" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="F80" t="s">
-        <v>183</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>201</v>
+        <v>166</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B81" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C81" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D81" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="E81" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="F81" t="s">
-        <v>188</v>
-      </c>
-      <c r="G81" t="s">
-        <v>161</v>
+        <v>164</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B82" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C82" t="s">
         <v>9</v>
       </c>
       <c r="D82" t="s">
-        <v>79</v>
+        <v>243</v>
       </c>
       <c r="E82" t="s">
-        <v>56</v>
+        <v>243</v>
       </c>
       <c r="F82" t="s">
-        <v>188</v>
-      </c>
-      <c r="G82" t="s">
-        <v>161</v>
+        <v>244</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B83" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C83" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D83" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E83" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="F83" t="s">
-        <v>188</v>
-      </c>
-      <c r="G83" t="s">
+        <v>197</v>
+      </c>
+      <c r="G83" s="1" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B84" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C84" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D84" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="E84" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F84" t="s">
-        <v>188</v>
-      </c>
-      <c r="G84" t="s">
+        <v>182</v>
+      </c>
+      <c r="G84" s="1" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B85" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C85" t="s">
         <v>9</v>
       </c>
       <c r="D85" t="s">
-        <v>203</v>
+        <v>69</v>
       </c>
       <c r="E85" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="F85" t="s">
-        <v>188</v>
-      </c>
-      <c r="G85" t="s">
+        <v>195</v>
+      </c>
+      <c r="G85" s="1" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B86" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C86" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D86" t="s">
-        <v>204</v>
+        <v>72</v>
       </c>
       <c r="E86" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="F86" t="s">
-        <v>188</v>
-      </c>
-      <c r="G86" t="s">
+        <v>196</v>
+      </c>
+      <c r="G86" s="1" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B87" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C87" t="s">
         <v>9</v>
       </c>
       <c r="D87" t="s">
-        <v>82</v>
+        <v>243</v>
       </c>
       <c r="E87" t="s">
-        <v>83</v>
+        <v>243</v>
       </c>
       <c r="F87" t="s">
-        <v>198</v>
+        <v>244</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>201</v>
@@ -3829,22 +3835,22 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B88" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C88" t="s">
         <v>9</v>
       </c>
       <c r="D88" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="E88" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="F88" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="G88" s="2" t="s">
         <v>201</v>
@@ -3852,22 +3858,22 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B89" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C89" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D89" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E89" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="F89" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G89" s="2" t="s">
         <v>201</v>
@@ -3875,22 +3881,22 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B90" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C90" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D90" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="E90" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="F90" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>201</v>
@@ -3907,16 +3913,16 @@
         <v>9</v>
       </c>
       <c r="D91" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E91" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="F91" t="s">
-        <v>198</v>
-      </c>
-      <c r="G91" s="2" t="s">
-        <v>201</v>
+        <v>188</v>
+      </c>
+      <c r="G91" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -3930,16 +3936,16 @@
         <v>9</v>
       </c>
       <c r="D92" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E92" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="F92" t="s">
-        <v>198</v>
-      </c>
-      <c r="G92" s="2" t="s">
-        <v>201</v>
+        <v>188</v>
+      </c>
+      <c r="G92" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
@@ -3953,16 +3959,16 @@
         <v>9</v>
       </c>
       <c r="D93" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E93" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="F93" t="s">
-        <v>198</v>
-      </c>
-      <c r="G93" s="2" t="s">
-        <v>201</v>
+        <v>188</v>
+      </c>
+      <c r="G93" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
@@ -3976,16 +3982,16 @@
         <v>9</v>
       </c>
       <c r="D94" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E94" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="F94" t="s">
-        <v>198</v>
-      </c>
-      <c r="G94" s="2" t="s">
-        <v>201</v>
+        <v>188</v>
+      </c>
+      <c r="G94" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
@@ -3999,16 +4005,16 @@
         <v>9</v>
       </c>
       <c r="D95" t="s">
-        <v>91</v>
+        <v>203</v>
       </c>
       <c r="E95" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="F95" t="s">
-        <v>198</v>
-      </c>
-      <c r="G95" s="2" t="s">
-        <v>201</v>
+        <v>188</v>
+      </c>
+      <c r="G95" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
@@ -4022,16 +4028,16 @@
         <v>9</v>
       </c>
       <c r="D96" t="s">
-        <v>92</v>
+        <v>204</v>
       </c>
       <c r="E96" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="F96" t="s">
-        <v>198</v>
-      </c>
-      <c r="G96" s="2" t="s">
-        <v>201</v>
+        <v>188</v>
+      </c>
+      <c r="G96" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -4045,7 +4051,7 @@
         <v>9</v>
       </c>
       <c r="D97" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="E97" t="s">
         <v>83</v>
@@ -4068,7 +4074,7 @@
         <v>9</v>
       </c>
       <c r="D98" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="E98" t="s">
         <v>83</v>
@@ -4091,7 +4097,7 @@
         <v>9</v>
       </c>
       <c r="D99" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="E99" t="s">
         <v>83</v>
@@ -4114,7 +4120,7 @@
         <v>9</v>
       </c>
       <c r="D100" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E100" t="s">
         <v>83</v>
@@ -4137,7 +4143,7 @@
         <v>9</v>
       </c>
       <c r="D101" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="E101" t="s">
         <v>83</v>
@@ -4160,7 +4166,7 @@
         <v>9</v>
       </c>
       <c r="D102" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="E102" t="s">
         <v>83</v>
@@ -4183,7 +4189,7 @@
         <v>9</v>
       </c>
       <c r="D103" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E103" t="s">
         <v>83</v>
@@ -4206,7 +4212,7 @@
         <v>9</v>
       </c>
       <c r="D104" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E104" t="s">
         <v>83</v>
@@ -4229,7 +4235,7 @@
         <v>9</v>
       </c>
       <c r="D105" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E105" t="s">
         <v>83</v>
@@ -4252,7 +4258,7 @@
         <v>9</v>
       </c>
       <c r="D106" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E106" t="s">
         <v>83</v>
@@ -4275,7 +4281,7 @@
         <v>9</v>
       </c>
       <c r="D107" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E107" t="s">
         <v>83</v>
@@ -4298,7 +4304,7 @@
         <v>9</v>
       </c>
       <c r="D108" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E108" t="s">
         <v>83</v>
@@ -4321,7 +4327,7 @@
         <v>9</v>
       </c>
       <c r="D109" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E109" t="s">
         <v>83</v>
@@ -4344,7 +4350,7 @@
         <v>9</v>
       </c>
       <c r="D110" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="E110" t="s">
         <v>83</v>
@@ -4367,7 +4373,7 @@
         <v>9</v>
       </c>
       <c r="D111" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="E111" t="s">
         <v>83</v>
@@ -4390,7 +4396,7 @@
         <v>9</v>
       </c>
       <c r="D112" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="E112" t="s">
         <v>83</v>
@@ -4413,7 +4419,7 @@
         <v>9</v>
       </c>
       <c r="D113" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E113" t="s">
         <v>83</v>
@@ -4436,7 +4442,7 @@
         <v>9</v>
       </c>
       <c r="D114" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E114" t="s">
         <v>83</v>
@@ -4459,7 +4465,7 @@
         <v>9</v>
       </c>
       <c r="D115" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="E115" t="s">
         <v>83</v>
@@ -4482,7 +4488,7 @@
         <v>9</v>
       </c>
       <c r="D116" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E116" t="s">
         <v>83</v>
@@ -4505,7 +4511,7 @@
         <v>9</v>
       </c>
       <c r="D117" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E117" t="s">
         <v>83</v>
@@ -4528,7 +4534,7 @@
         <v>9</v>
       </c>
       <c r="D118" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E118" t="s">
         <v>83</v>
@@ -4551,7 +4557,7 @@
         <v>9</v>
       </c>
       <c r="D119" t="s">
-        <v>205</v>
+        <v>103</v>
       </c>
       <c r="E119" t="s">
         <v>83</v>
@@ -4574,7 +4580,7 @@
         <v>9</v>
       </c>
       <c r="D120" t="s">
-        <v>206</v>
+        <v>80</v>
       </c>
       <c r="E120" t="s">
         <v>83</v>
@@ -4597,7 +4603,7 @@
         <v>9</v>
       </c>
       <c r="D121" t="s">
-        <v>207</v>
+        <v>104</v>
       </c>
       <c r="E121" t="s">
         <v>83</v>
@@ -4620,7 +4626,7 @@
         <v>9</v>
       </c>
       <c r="D122" t="s">
-        <v>208</v>
+        <v>105</v>
       </c>
       <c r="E122" t="s">
         <v>83</v>
@@ -4643,7 +4649,7 @@
         <v>9</v>
       </c>
       <c r="D123" t="s">
-        <v>209</v>
+        <v>106</v>
       </c>
       <c r="E123" t="s">
         <v>83</v>
@@ -4666,7 +4672,7 @@
         <v>9</v>
       </c>
       <c r="D124" t="s">
-        <v>210</v>
+        <v>107</v>
       </c>
       <c r="E124" t="s">
         <v>83</v>
@@ -4689,7 +4695,7 @@
         <v>9</v>
       </c>
       <c r="D125" t="s">
-        <v>211</v>
+        <v>81</v>
       </c>
       <c r="E125" t="s">
         <v>83</v>
@@ -4712,7 +4718,7 @@
         <v>9</v>
       </c>
       <c r="D126" t="s">
-        <v>203</v>
+        <v>108</v>
       </c>
       <c r="E126" t="s">
         <v>83</v>
@@ -4735,7 +4741,7 @@
         <v>9</v>
       </c>
       <c r="D127" t="s">
-        <v>212</v>
+        <v>109</v>
       </c>
       <c r="E127" t="s">
         <v>83</v>
@@ -4758,7 +4764,7 @@
         <v>9</v>
       </c>
       <c r="D128" t="s">
-        <v>213</v>
+        <v>110</v>
       </c>
       <c r="E128" t="s">
         <v>83</v>
@@ -4781,7 +4787,7 @@
         <v>9</v>
       </c>
       <c r="D129" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E129" t="s">
         <v>83</v>
@@ -4804,7 +4810,7 @@
         <v>9</v>
       </c>
       <c r="D130" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E130" t="s">
         <v>83</v>
@@ -4827,7 +4833,7 @@
         <v>9</v>
       </c>
       <c r="D131" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="E131" t="s">
         <v>83</v>
@@ -4850,13 +4856,13 @@
         <v>9</v>
       </c>
       <c r="D132" t="s">
-        <v>109</v>
+        <v>208</v>
       </c>
       <c r="E132" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="F132" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="G132" s="2" t="s">
         <v>201</v>
@@ -4873,13 +4879,13 @@
         <v>9</v>
       </c>
       <c r="D133" t="s">
-        <v>85</v>
+        <v>209</v>
       </c>
       <c r="E133" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="F133" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="G133" s="2" t="s">
         <v>201</v>
@@ -4896,13 +4902,13 @@
         <v>9</v>
       </c>
       <c r="D134" t="s">
-        <v>89</v>
+        <v>210</v>
       </c>
       <c r="E134" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="F134" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="G134" s="2" t="s">
         <v>201</v>
@@ -4919,13 +4925,13 @@
         <v>9</v>
       </c>
       <c r="D135" t="s">
-        <v>90</v>
+        <v>211</v>
       </c>
       <c r="E135" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="F135" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="G135" s="2" t="s">
         <v>201</v>
@@ -4942,13 +4948,13 @@
         <v>9</v>
       </c>
       <c r="D136" t="s">
-        <v>79</v>
+        <v>203</v>
       </c>
       <c r="E136" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="F136" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="G136" s="2" t="s">
         <v>201</v>
@@ -4965,13 +4971,13 @@
         <v>9</v>
       </c>
       <c r="D137" t="s">
-        <v>99</v>
+        <v>212</v>
       </c>
       <c r="E137" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="F137" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="G137" s="2" t="s">
         <v>201</v>
@@ -4988,13 +4994,13 @@
         <v>9</v>
       </c>
       <c r="D138" t="s">
-        <v>80</v>
+        <v>213</v>
       </c>
       <c r="E138" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="F138" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="G138" s="2" t="s">
         <v>201</v>
@@ -5011,13 +5017,13 @@
         <v>9</v>
       </c>
       <c r="D139" t="s">
-        <v>104</v>
+        <v>214</v>
       </c>
       <c r="E139" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="F139" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="G139" s="2" t="s">
         <v>201</v>
@@ -5034,13 +5040,13 @@
         <v>9</v>
       </c>
       <c r="D140" t="s">
-        <v>109</v>
+        <v>204</v>
       </c>
       <c r="E140" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="F140" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="G140" s="2" t="s">
         <v>201</v>
@@ -5057,13 +5063,13 @@
         <v>9</v>
       </c>
       <c r="D141" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="E141" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="F141" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="G141" s="2" t="s">
         <v>201</v>
@@ -5080,13 +5086,13 @@
         <v>9</v>
       </c>
       <c r="D142" t="s">
-        <v>203</v>
+        <v>109</v>
       </c>
       <c r="E142" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="F142" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
       <c r="G142" s="2" t="s">
         <v>201</v>
@@ -5103,7 +5109,7 @@
         <v>9</v>
       </c>
       <c r="D143" t="s">
-        <v>216</v>
+        <v>85</v>
       </c>
       <c r="E143" t="s">
         <v>19</v>
@@ -5126,13 +5132,13 @@
         <v>9</v>
       </c>
       <c r="D144" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E144" t="s">
-        <v>111</v>
+        <v>19</v>
       </c>
       <c r="F144" t="s">
-        <v>199</v>
+        <v>166</v>
       </c>
       <c r="G144" s="2" t="s">
         <v>201</v>
@@ -5149,13 +5155,13 @@
         <v>9</v>
       </c>
       <c r="D145" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E145" t="s">
-        <v>111</v>
+        <v>19</v>
       </c>
       <c r="F145" t="s">
-        <v>199</v>
+        <v>166</v>
       </c>
       <c r="G145" s="2" t="s">
         <v>201</v>
@@ -5172,13 +5178,13 @@
         <v>9</v>
       </c>
       <c r="D146" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E146" t="s">
-        <v>111</v>
+        <v>19</v>
       </c>
       <c r="F146" t="s">
-        <v>199</v>
+        <v>166</v>
       </c>
       <c r="G146" s="2" t="s">
         <v>201</v>
@@ -5195,13 +5201,13 @@
         <v>9</v>
       </c>
       <c r="D147" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E147" t="s">
-        <v>111</v>
+        <v>19</v>
       </c>
       <c r="F147" t="s">
-        <v>199</v>
+        <v>166</v>
       </c>
       <c r="G147" s="2" t="s">
         <v>201</v>
@@ -5218,13 +5224,13 @@
         <v>9</v>
       </c>
       <c r="D148" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="E148" t="s">
-        <v>111</v>
+        <v>19</v>
       </c>
       <c r="F148" t="s">
-        <v>199</v>
+        <v>166</v>
       </c>
       <c r="G148" s="2" t="s">
         <v>201</v>
@@ -5241,13 +5247,13 @@
         <v>9</v>
       </c>
       <c r="D149" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="E149" t="s">
-        <v>111</v>
+        <v>19</v>
       </c>
       <c r="F149" t="s">
-        <v>199</v>
+        <v>166</v>
       </c>
       <c r="G149" s="2" t="s">
         <v>201</v>
@@ -5264,13 +5270,13 @@
         <v>9</v>
       </c>
       <c r="D150" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="E150" t="s">
-        <v>111</v>
+        <v>19</v>
       </c>
       <c r="F150" t="s">
-        <v>199</v>
+        <v>166</v>
       </c>
       <c r="G150" s="2" t="s">
         <v>201</v>
@@ -5287,13 +5293,13 @@
         <v>9</v>
       </c>
       <c r="D151" t="s">
-        <v>102</v>
+        <v>207</v>
       </c>
       <c r="E151" t="s">
-        <v>111</v>
+        <v>19</v>
       </c>
       <c r="F151" t="s">
-        <v>199</v>
+        <v>166</v>
       </c>
       <c r="G151" s="2" t="s">
         <v>201</v>
@@ -5310,13 +5316,13 @@
         <v>9</v>
       </c>
       <c r="D152" t="s">
-        <v>103</v>
+        <v>203</v>
       </c>
       <c r="E152" t="s">
-        <v>111</v>
+        <v>19</v>
       </c>
       <c r="F152" t="s">
-        <v>199</v>
+        <v>166</v>
       </c>
       <c r="G152" s="2" t="s">
         <v>201</v>
@@ -5333,13 +5339,13 @@
         <v>9</v>
       </c>
       <c r="D153" t="s">
-        <v>110</v>
+        <v>216</v>
       </c>
       <c r="E153" t="s">
-        <v>111</v>
+        <v>19</v>
       </c>
       <c r="F153" t="s">
-        <v>199</v>
+        <v>166</v>
       </c>
       <c r="G153" s="2" t="s">
         <v>201</v>
@@ -5356,7 +5362,7 @@
         <v>9</v>
       </c>
       <c r="D154" t="s">
-        <v>205</v>
+        <v>84</v>
       </c>
       <c r="E154" t="s">
         <v>111</v>
@@ -5379,7 +5385,7 @@
         <v>9</v>
       </c>
       <c r="D155" t="s">
-        <v>206</v>
+        <v>85</v>
       </c>
       <c r="E155" t="s">
         <v>111</v>
@@ -5402,7 +5408,7 @@
         <v>9</v>
       </c>
       <c r="D156" t="s">
-        <v>207</v>
+        <v>86</v>
       </c>
       <c r="E156" t="s">
         <v>111</v>
@@ -5425,7 +5431,7 @@
         <v>9</v>
       </c>
       <c r="D157" t="s">
-        <v>208</v>
+        <v>97</v>
       </c>
       <c r="E157" t="s">
         <v>111</v>
@@ -5448,7 +5454,7 @@
         <v>9</v>
       </c>
       <c r="D158" t="s">
-        <v>210</v>
+        <v>98</v>
       </c>
       <c r="E158" t="s">
         <v>111</v>
@@ -5471,7 +5477,7 @@
         <v>9</v>
       </c>
       <c r="D159" t="s">
-        <v>211</v>
+        <v>99</v>
       </c>
       <c r="E159" t="s">
         <v>111</v>
@@ -5491,19 +5497,19 @@
         <v>77</v>
       </c>
       <c r="C160" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D160" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="E160" t="s">
-        <v>12</v>
+        <v>111</v>
       </c>
       <c r="F160" t="s">
-        <v>163</v>
-      </c>
-      <c r="G160" t="s">
-        <v>161</v>
+        <v>199</v>
+      </c>
+      <c r="G160" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.3">
@@ -5514,19 +5520,19 @@
         <v>77</v>
       </c>
       <c r="C161" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D161" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="E161" t="s">
-        <v>12</v>
+        <v>111</v>
       </c>
       <c r="F161" t="s">
-        <v>163</v>
-      </c>
-      <c r="G161" t="s">
-        <v>161</v>
+        <v>199</v>
+      </c>
+      <c r="G161" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.3">
@@ -5537,16 +5543,16 @@
         <v>77</v>
       </c>
       <c r="C162" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D162" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="E162" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F162" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G162" s="2" t="s">
         <v>201</v>
@@ -5560,16 +5566,16 @@
         <v>77</v>
       </c>
       <c r="C163" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D163" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E163" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F163" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G163" s="2" t="s">
         <v>201</v>
@@ -5583,16 +5589,16 @@
         <v>77</v>
       </c>
       <c r="C164" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D164" t="s">
-        <v>117</v>
+        <v>205</v>
       </c>
       <c r="E164" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F164" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G164" s="2" t="s">
         <v>201</v>
@@ -5606,16 +5612,16 @@
         <v>77</v>
       </c>
       <c r="C165" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D165" t="s">
-        <v>118</v>
+        <v>206</v>
       </c>
       <c r="E165" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F165" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G165" s="2" t="s">
         <v>201</v>
@@ -5629,16 +5635,16 @@
         <v>77</v>
       </c>
       <c r="C166" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D166" t="s">
-        <v>119</v>
+        <v>207</v>
       </c>
       <c r="E166" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F166" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G166" s="2" t="s">
         <v>201</v>
@@ -5652,16 +5658,16 @@
         <v>77</v>
       </c>
       <c r="C167" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D167" t="s">
-        <v>120</v>
+        <v>208</v>
       </c>
       <c r="E167" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F167" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G167" s="2" t="s">
         <v>201</v>
@@ -5675,19 +5681,19 @@
         <v>77</v>
       </c>
       <c r="C168" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D168" t="s">
-        <v>58</v>
+        <v>210</v>
       </c>
       <c r="E168" t="s">
-        <v>58</v>
+        <v>111</v>
       </c>
       <c r="F168" t="s">
-        <v>189</v>
-      </c>
-      <c r="G168" t="s">
-        <v>161</v>
+        <v>199</v>
+      </c>
+      <c r="G168" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.3">
@@ -5698,16 +5704,16 @@
         <v>77</v>
       </c>
       <c r="C169" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D169" t="s">
-        <v>121</v>
+        <v>211</v>
       </c>
       <c r="E169" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="F169" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="G169" s="2" t="s">
         <v>201</v>
@@ -5724,16 +5730,16 @@
         <v>8</v>
       </c>
       <c r="D170" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E170" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="F170" t="s">
-        <v>179</v>
-      </c>
-      <c r="G170" s="2" t="s">
-        <v>201</v>
+        <v>163</v>
+      </c>
+      <c r="G170" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.3">
@@ -5747,16 +5753,16 @@
         <v>8</v>
       </c>
       <c r="D171" t="s">
-        <v>217</v>
+        <v>113</v>
       </c>
       <c r="E171" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="F171" t="s">
-        <v>179</v>
-      </c>
-      <c r="G171" s="2" t="s">
-        <v>201</v>
+        <v>163</v>
+      </c>
+      <c r="G171" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.3">
@@ -5770,13 +5776,13 @@
         <v>8</v>
       </c>
       <c r="D172" t="s">
-        <v>218</v>
+        <v>114</v>
       </c>
       <c r="E172" t="s">
-        <v>44</v>
+        <v>115</v>
       </c>
       <c r="F172" t="s">
-        <v>179</v>
+        <v>200</v>
       </c>
       <c r="G172" s="2" t="s">
         <v>201</v>
@@ -5793,13 +5799,13 @@
         <v>8</v>
       </c>
       <c r="D173" t="s">
-        <v>219</v>
+        <v>116</v>
       </c>
       <c r="E173" t="s">
-        <v>44</v>
+        <v>115</v>
       </c>
       <c r="F173" t="s">
-        <v>179</v>
+        <v>200</v>
       </c>
       <c r="G173" s="2" t="s">
         <v>201</v>
@@ -5816,13 +5822,13 @@
         <v>8</v>
       </c>
       <c r="D174" t="s">
-        <v>220</v>
+        <v>117</v>
       </c>
       <c r="E174" t="s">
-        <v>44</v>
+        <v>115</v>
       </c>
       <c r="F174" t="s">
-        <v>179</v>
+        <v>200</v>
       </c>
       <c r="G174" s="2" t="s">
         <v>201</v>
@@ -5839,13 +5845,13 @@
         <v>8</v>
       </c>
       <c r="D175" t="s">
-        <v>221</v>
+        <v>118</v>
       </c>
       <c r="E175" t="s">
-        <v>44</v>
+        <v>115</v>
       </c>
       <c r="F175" t="s">
-        <v>179</v>
+        <v>200</v>
       </c>
       <c r="G175" s="2" t="s">
         <v>201</v>
@@ -5865,13 +5871,13 @@
         <v>119</v>
       </c>
       <c r="E176" t="s">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="F176" t="s">
-        <v>180</v>
-      </c>
-      <c r="G176" s="1" t="s">
-        <v>161</v>
+        <v>200</v>
+      </c>
+      <c r="G176" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.3">
@@ -5882,19 +5888,19 @@
         <v>77</v>
       </c>
       <c r="C177" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D177" t="s">
-        <v>79</v>
+        <v>120</v>
       </c>
       <c r="E177" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
       <c r="F177" t="s">
-        <v>186</v>
-      </c>
-      <c r="G177" t="s">
-        <v>161</v>
+        <v>200</v>
+      </c>
+      <c r="G177" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.3">
@@ -5905,16 +5911,16 @@
         <v>77</v>
       </c>
       <c r="C178" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D178" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="E178" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F178" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="G178" t="s">
         <v>161</v>
@@ -5928,19 +5934,19 @@
         <v>77</v>
       </c>
       <c r="C179" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D179" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="E179" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="F179" t="s">
-        <v>186</v>
-      </c>
-      <c r="G179" t="s">
-        <v>161</v>
+        <v>179</v>
+      </c>
+      <c r="G179" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.3">
@@ -5951,19 +5957,19 @@
         <v>77</v>
       </c>
       <c r="C180" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D180" t="s">
-        <v>208</v>
+        <v>122</v>
       </c>
       <c r="E180" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="F180" t="s">
-        <v>186</v>
-      </c>
-      <c r="G180" t="s">
-        <v>161</v>
+        <v>179</v>
+      </c>
+      <c r="G180" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.3">
@@ -5977,13 +5983,13 @@
         <v>8</v>
       </c>
       <c r="D181" t="s">
-        <v>123</v>
+        <v>217</v>
       </c>
       <c r="E181" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F181" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G181" s="2" t="s">
         <v>201</v>
@@ -6000,13 +6006,13 @@
         <v>8</v>
       </c>
       <c r="D182" t="s">
-        <v>117</v>
+        <v>218</v>
       </c>
       <c r="E182" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F182" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G182" s="2" t="s">
         <v>201</v>
@@ -6023,13 +6029,13 @@
         <v>8</v>
       </c>
       <c r="D183" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E183" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F183" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G183" s="2" t="s">
         <v>201</v>
@@ -6043,16 +6049,16 @@
         <v>77</v>
       </c>
       <c r="C184" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D184" t="s">
-        <v>90</v>
+        <v>220</v>
       </c>
       <c r="E184" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F184" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G184" s="2" t="s">
         <v>201</v>
@@ -6066,16 +6072,16 @@
         <v>77</v>
       </c>
       <c r="C185" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D185" t="s">
-        <v>97</v>
+        <v>221</v>
       </c>
       <c r="E185" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F185" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G185" s="2" t="s">
         <v>201</v>
@@ -6089,19 +6095,19 @@
         <v>77</v>
       </c>
       <c r="C186" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D186" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="E186" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F186" t="s">
-        <v>182</v>
-      </c>
-      <c r="G186" s="2" t="s">
-        <v>201</v>
+        <v>180</v>
+      </c>
+      <c r="G186" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.3">
@@ -6115,16 +6121,16 @@
         <v>9</v>
       </c>
       <c r="D187" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="E187" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F187" t="s">
-        <v>182</v>
-      </c>
-      <c r="G187" s="2" t="s">
-        <v>201</v>
+        <v>186</v>
+      </c>
+      <c r="G187" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.3">
@@ -6135,18 +6141,18 @@
         <v>77</v>
       </c>
       <c r="C188" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D188" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="E188" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F188" t="s">
-        <v>182</v>
-      </c>
-      <c r="G188" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G188" t="s">
         <v>161</v>
       </c>
     </row>
@@ -6161,16 +6167,16 @@
         <v>9</v>
       </c>
       <c r="D189" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E189" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F189" t="s">
-        <v>182</v>
-      </c>
-      <c r="G189" s="2" t="s">
-        <v>201</v>
+        <v>186</v>
+      </c>
+      <c r="G189" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.3">
@@ -6184,16 +6190,16 @@
         <v>9</v>
       </c>
       <c r="D190" t="s">
-        <v>102</v>
+        <v>208</v>
       </c>
       <c r="E190" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F190" t="s">
-        <v>182</v>
-      </c>
-      <c r="G190" s="2" t="s">
-        <v>201</v>
+        <v>186</v>
+      </c>
+      <c r="G190" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.3">
@@ -6204,16 +6210,16 @@
         <v>77</v>
       </c>
       <c r="C191" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D191" t="s">
-        <v>80</v>
+        <v>123</v>
       </c>
       <c r="E191" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F191" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G191" s="2" t="s">
         <v>201</v>
@@ -6227,16 +6233,16 @@
         <v>77</v>
       </c>
       <c r="C192" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D192" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="E192" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F192" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G192" s="2" t="s">
         <v>201</v>
@@ -6250,16 +6256,16 @@
         <v>77</v>
       </c>
       <c r="C193" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D193" t="s">
-        <v>106</v>
+        <v>222</v>
       </c>
       <c r="E193" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F193" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G193" s="2" t="s">
         <v>201</v>
@@ -6276,7 +6282,7 @@
         <v>9</v>
       </c>
       <c r="D194" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="E194" t="s">
         <v>48</v>
@@ -6299,7 +6305,7 @@
         <v>9</v>
       </c>
       <c r="D195" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="E195" t="s">
         <v>48</v>
@@ -6322,7 +6328,7 @@
         <v>9</v>
       </c>
       <c r="D196" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="E196" t="s">
         <v>48</v>
@@ -6345,7 +6351,7 @@
         <v>9</v>
       </c>
       <c r="D197" t="s">
-        <v>203</v>
+        <v>100</v>
       </c>
       <c r="E197" t="s">
         <v>48</v>
@@ -6365,10 +6371,10 @@
         <v>77</v>
       </c>
       <c r="C198" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D198" t="s">
-        <v>215</v>
+        <v>124</v>
       </c>
       <c r="E198" t="s">
         <v>48</v>
@@ -6376,8 +6382,8 @@
       <c r="F198" t="s">
         <v>182</v>
       </c>
-      <c r="G198" s="2" t="s">
-        <v>201</v>
+      <c r="G198" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.3">
@@ -6388,16 +6394,16 @@
         <v>77</v>
       </c>
       <c r="C199" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D199" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="E199" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F199" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G199" s="2" t="s">
         <v>201</v>
@@ -6411,16 +6417,16 @@
         <v>77</v>
       </c>
       <c r="C200" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D200" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="E200" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F200" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G200" s="2" t="s">
         <v>201</v>
@@ -6434,16 +6440,16 @@
         <v>77</v>
       </c>
       <c r="C201" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D201" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="E201" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F201" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G201" s="2" t="s">
         <v>201</v>
@@ -6457,16 +6463,16 @@
         <v>77</v>
       </c>
       <c r="C202" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D202" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="E202" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F202" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G202" s="2" t="s">
         <v>201</v>
@@ -6480,16 +6486,16 @@
         <v>77</v>
       </c>
       <c r="C203" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D203" t="s">
-        <v>222</v>
+        <v>106</v>
       </c>
       <c r="E203" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F203" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G203" s="2" t="s">
         <v>201</v>
@@ -6503,16 +6509,16 @@
         <v>77</v>
       </c>
       <c r="C204" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D204" t="s">
-        <v>223</v>
+        <v>81</v>
       </c>
       <c r="E204" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F204" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G204" s="2" t="s">
         <v>201</v>
@@ -6526,16 +6532,16 @@
         <v>77</v>
       </c>
       <c r="C205" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D205" t="s">
-        <v>218</v>
+        <v>108</v>
       </c>
       <c r="E205" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F205" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G205" s="2" t="s">
         <v>201</v>
@@ -6549,16 +6555,16 @@
         <v>77</v>
       </c>
       <c r="C206" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D206" t="s">
-        <v>219</v>
+        <v>109</v>
       </c>
       <c r="E206" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F206" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G206" s="2" t="s">
         <v>201</v>
@@ -6572,16 +6578,16 @@
         <v>77</v>
       </c>
       <c r="C207" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D207" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="E207" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F207" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G207" s="2" t="s">
         <v>201</v>
@@ -6595,16 +6601,16 @@
         <v>77</v>
       </c>
       <c r="C208" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D208" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="E208" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F208" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G208" s="2" t="s">
         <v>201</v>
@@ -6615,19 +6621,19 @@
         <v>76</v>
       </c>
       <c r="B209" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="C209" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D209" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="E209" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="F209" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="G209" s="2" t="s">
         <v>201</v>
@@ -6638,19 +6644,19 @@
         <v>76</v>
       </c>
       <c r="B210" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="C210" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D210" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="E210" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="F210" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="G210" s="2" t="s">
         <v>201</v>
@@ -6661,19 +6667,19 @@
         <v>76</v>
       </c>
       <c r="B211" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="C211" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D211" t="s">
-        <v>225</v>
+        <v>125</v>
       </c>
       <c r="E211" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="F211" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="G211" s="2" t="s">
         <v>201</v>
@@ -6684,19 +6690,19 @@
         <v>76</v>
       </c>
       <c r="B212" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="C212" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D212" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E212" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="F212" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="G212" s="2" t="s">
         <v>201</v>
@@ -6707,19 +6713,19 @@
         <v>76</v>
       </c>
       <c r="B213" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="C213" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D213" t="s">
-        <v>131</v>
+        <v>222</v>
       </c>
       <c r="E213" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="F213" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="G213" s="2" t="s">
         <v>201</v>
@@ -6730,19 +6736,19 @@
         <v>76</v>
       </c>
       <c r="B214" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="C214" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D214" t="s">
-        <v>132</v>
+        <v>223</v>
       </c>
       <c r="E214" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="F214" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="G214" s="2" t="s">
         <v>201</v>
@@ -6753,19 +6759,19 @@
         <v>76</v>
       </c>
       <c r="B215" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="C215" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D215" t="s">
-        <v>133</v>
+        <v>218</v>
       </c>
       <c r="E215" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="F215" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="G215" s="2" t="s">
         <v>201</v>
@@ -6776,19 +6782,19 @@
         <v>76</v>
       </c>
       <c r="B216" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="C216" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D216" t="s">
-        <v>134</v>
+        <v>219</v>
       </c>
       <c r="E216" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="F216" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="G216" s="2" t="s">
         <v>201</v>
@@ -6799,19 +6805,19 @@
         <v>76</v>
       </c>
       <c r="B217" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="C217" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D217" t="s">
-        <v>135</v>
+        <v>220</v>
       </c>
       <c r="E217" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="F217" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="G217" s="2" t="s">
         <v>201</v>
@@ -6822,19 +6828,19 @@
         <v>76</v>
       </c>
       <c r="B218" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="C218" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D218" t="s">
-        <v>136</v>
+        <v>224</v>
       </c>
       <c r="E218" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="F218" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="G218" s="2" t="s">
         <v>201</v>
@@ -6851,7 +6857,7 @@
         <v>9</v>
       </c>
       <c r="D219" t="s">
-        <v>226</v>
+        <v>128</v>
       </c>
       <c r="E219" t="s">
         <v>83</v>
@@ -6874,7 +6880,7 @@
         <v>9</v>
       </c>
       <c r="D220" t="s">
-        <v>227</v>
+        <v>129</v>
       </c>
       <c r="E220" t="s">
         <v>83</v>
@@ -6897,7 +6903,7 @@
         <v>9</v>
       </c>
       <c r="D221" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E221" t="s">
         <v>83</v>
@@ -6920,7 +6926,7 @@
         <v>9</v>
       </c>
       <c r="D222" t="s">
-        <v>229</v>
+        <v>130</v>
       </c>
       <c r="E222" t="s">
         <v>83</v>
@@ -6943,13 +6949,13 @@
         <v>9</v>
       </c>
       <c r="D223" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E223" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="F223" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="G223" s="2" t="s">
         <v>201</v>
@@ -6966,13 +6972,13 @@
         <v>9</v>
       </c>
       <c r="D224" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E224" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="F224" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="G224" s="2" t="s">
         <v>201</v>
@@ -6989,13 +6995,13 @@
         <v>9</v>
       </c>
       <c r="D225" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="E225" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="F225" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="G225" s="2" t="s">
         <v>201</v>
@@ -7012,13 +7018,13 @@
         <v>9</v>
       </c>
       <c r="D226" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E226" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="F226" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G226" s="2" t="s">
         <v>201</v>
@@ -7032,19 +7038,19 @@
         <v>127</v>
       </c>
       <c r="C227" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D227" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E227" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="F227" t="s">
-        <v>199</v>
-      </c>
-      <c r="G227" s="1" t="s">
-        <v>161</v>
+        <v>198</v>
+      </c>
+      <c r="G227" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.3">
@@ -7058,13 +7064,13 @@
         <v>9</v>
       </c>
       <c r="D228" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E228" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="F228" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G228" s="2" t="s">
         <v>201</v>
@@ -7078,19 +7084,19 @@
         <v>127</v>
       </c>
       <c r="C229" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D229" t="s">
-        <v>143</v>
+        <v>226</v>
       </c>
       <c r="E229" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="F229" t="s">
-        <v>199</v>
-      </c>
-      <c r="G229" s="1" t="s">
-        <v>161</v>
+        <v>198</v>
+      </c>
+      <c r="G229" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.3">
@@ -7104,13 +7110,13 @@
         <v>9</v>
       </c>
       <c r="D230" t="s">
-        <v>144</v>
+        <v>227</v>
       </c>
       <c r="E230" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="F230" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G230" s="2" t="s">
         <v>201</v>
@@ -7127,13 +7133,13 @@
         <v>9</v>
       </c>
       <c r="D231" t="s">
-        <v>129</v>
+        <v>228</v>
       </c>
       <c r="E231" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="F231" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G231" s="2" t="s">
         <v>201</v>
@@ -7150,13 +7156,13 @@
         <v>9</v>
       </c>
       <c r="D232" t="s">
-        <v>145</v>
+        <v>229</v>
       </c>
       <c r="E232" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="F232" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G232" s="2" t="s">
         <v>201</v>
@@ -7173,13 +7179,13 @@
         <v>9</v>
       </c>
       <c r="D233" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E233" t="s">
-        <v>111</v>
+        <v>51</v>
       </c>
       <c r="F233" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="G233" s="2" t="s">
         <v>201</v>
@@ -7196,13 +7202,13 @@
         <v>9</v>
       </c>
       <c r="D234" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="E234" t="s">
-        <v>111</v>
+        <v>51</v>
       </c>
       <c r="F234" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="G234" s="2" t="s">
         <v>201</v>
@@ -7219,13 +7225,13 @@
         <v>9</v>
       </c>
       <c r="D235" t="s">
-        <v>131</v>
+        <v>19</v>
       </c>
       <c r="E235" t="s">
-        <v>111</v>
+        <v>19</v>
       </c>
       <c r="F235" t="s">
-        <v>199</v>
+        <v>166</v>
       </c>
       <c r="G235" s="2" t="s">
         <v>201</v>
@@ -7242,7 +7248,7 @@
         <v>9</v>
       </c>
       <c r="D236" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E236" t="s">
         <v>111</v>
@@ -7262,10 +7268,10 @@
         <v>127</v>
       </c>
       <c r="C237" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D237" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E237" t="s">
         <v>111</v>
@@ -7273,8 +7279,8 @@
       <c r="F237" t="s">
         <v>199</v>
       </c>
-      <c r="G237" s="2" t="s">
-        <v>201</v>
+      <c r="G237" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.3">
@@ -7288,7 +7294,7 @@
         <v>9</v>
       </c>
       <c r="D238" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E238" t="s">
         <v>111</v>
@@ -7308,10 +7314,10 @@
         <v>127</v>
       </c>
       <c r="C239" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D239" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="E239" t="s">
         <v>111</v>
@@ -7319,8 +7325,8 @@
       <c r="F239" t="s">
         <v>199</v>
       </c>
-      <c r="G239" s="2" t="s">
-        <v>201</v>
+      <c r="G239" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.3">
@@ -7334,7 +7340,7 @@
         <v>9</v>
       </c>
       <c r="D240" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E240" t="s">
         <v>111</v>
@@ -7357,7 +7363,7 @@
         <v>9</v>
       </c>
       <c r="D241" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="E241" t="s">
         <v>111</v>
@@ -7380,7 +7386,7 @@
         <v>9</v>
       </c>
       <c r="D242" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="E242" t="s">
         <v>111</v>
@@ -7403,7 +7409,7 @@
         <v>9</v>
       </c>
       <c r="D243" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="E243" t="s">
         <v>111</v>
@@ -7426,7 +7432,7 @@
         <v>9</v>
       </c>
       <c r="D244" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E244" t="s">
         <v>111</v>
@@ -7449,7 +7455,7 @@
         <v>9</v>
       </c>
       <c r="D245" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="E245" t="s">
         <v>111</v>
@@ -7472,7 +7478,7 @@
         <v>9</v>
       </c>
       <c r="D246" t="s">
-        <v>230</v>
+        <v>132</v>
       </c>
       <c r="E246" t="s">
         <v>111</v>
@@ -7495,7 +7501,7 @@
         <v>9</v>
       </c>
       <c r="D247" t="s">
-        <v>231</v>
+        <v>146</v>
       </c>
       <c r="E247" t="s">
         <v>111</v>
@@ -7518,7 +7524,7 @@
         <v>9</v>
       </c>
       <c r="D248" t="s">
-        <v>232</v>
+        <v>147</v>
       </c>
       <c r="E248" t="s">
         <v>111</v>
@@ -7541,7 +7547,7 @@
         <v>9</v>
       </c>
       <c r="D249" t="s">
-        <v>233</v>
+        <v>134</v>
       </c>
       <c r="E249" t="s">
         <v>111</v>
@@ -7564,7 +7570,7 @@
         <v>9</v>
       </c>
       <c r="D250" t="s">
-        <v>234</v>
+        <v>148</v>
       </c>
       <c r="E250" t="s">
         <v>111</v>
@@ -7587,7 +7593,7 @@
         <v>9</v>
       </c>
       <c r="D251" t="s">
-        <v>235</v>
+        <v>149</v>
       </c>
       <c r="E251" t="s">
         <v>111</v>
@@ -7610,7 +7616,7 @@
         <v>9</v>
       </c>
       <c r="D252" t="s">
-        <v>226</v>
+        <v>135</v>
       </c>
       <c r="E252" t="s">
         <v>111</v>
@@ -7633,7 +7639,7 @@
         <v>9</v>
       </c>
       <c r="D253" t="s">
-        <v>227</v>
+        <v>150</v>
       </c>
       <c r="E253" t="s">
         <v>111</v>
@@ -7656,7 +7662,7 @@
         <v>9</v>
       </c>
       <c r="D254" t="s">
-        <v>229</v>
+        <v>136</v>
       </c>
       <c r="E254" t="s">
         <v>111</v>
@@ -7676,19 +7682,19 @@
         <v>127</v>
       </c>
       <c r="C255" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D255" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="E255" t="s">
-        <v>12</v>
+        <v>111</v>
       </c>
       <c r="F255" t="s">
-        <v>163</v>
-      </c>
-      <c r="G255" t="s">
-        <v>161</v>
+        <v>199</v>
+      </c>
+      <c r="G255" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.3">
@@ -7699,16 +7705,16 @@
         <v>127</v>
       </c>
       <c r="C256" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D256" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E256" t="s">
-        <v>34</v>
+        <v>111</v>
       </c>
       <c r="F256" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="G256" s="2" t="s">
         <v>201</v>
@@ -7722,16 +7728,16 @@
         <v>127</v>
       </c>
       <c r="C257" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D257" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E257" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="F257" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="G257" s="2" t="s">
         <v>201</v>
@@ -7745,16 +7751,16 @@
         <v>127</v>
       </c>
       <c r="C258" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D258" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E258" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="F258" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="G258" s="2" t="s">
         <v>201</v>
@@ -7768,19 +7774,19 @@
         <v>127</v>
       </c>
       <c r="C259" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D259" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="E259" t="s">
-        <v>45</v>
+        <v>111</v>
       </c>
       <c r="F259" t="s">
-        <v>180</v>
-      </c>
-      <c r="G259" s="1" t="s">
-        <v>161</v>
+        <v>199</v>
+      </c>
+      <c r="G259" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.3">
@@ -7791,19 +7797,19 @@
         <v>127</v>
       </c>
       <c r="C260" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D260" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E260" t="s">
-        <v>45</v>
+        <v>111</v>
       </c>
       <c r="F260" t="s">
-        <v>180</v>
-      </c>
-      <c r="G260" s="1" t="s">
-        <v>161</v>
+        <v>199</v>
+      </c>
+      <c r="G260" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.3">
@@ -7817,16 +7823,16 @@
         <v>9</v>
       </c>
       <c r="D261" t="s">
-        <v>153</v>
+        <v>235</v>
       </c>
       <c r="E261" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="F261" t="s">
-        <v>181</v>
-      </c>
-      <c r="G261" s="1" t="s">
-        <v>161</v>
+        <v>199</v>
+      </c>
+      <c r="G261" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.3">
@@ -7837,16 +7843,16 @@
         <v>127</v>
       </c>
       <c r="C262" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D262" t="s">
-        <v>154</v>
+        <v>226</v>
       </c>
       <c r="E262" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="F262" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="G262" s="2" t="s">
         <v>201</v>
@@ -7860,16 +7866,16 @@
         <v>127</v>
       </c>
       <c r="C263" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D263" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="E263" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="F263" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="G263" s="2" t="s">
         <v>201</v>
@@ -7886,13 +7892,13 @@
         <v>9</v>
       </c>
       <c r="D264" t="s">
-        <v>133</v>
+        <v>229</v>
       </c>
       <c r="E264" t="s">
-        <v>48</v>
+        <v>111</v>
       </c>
       <c r="F264" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
       <c r="G264" s="2" t="s">
         <v>201</v>
@@ -7906,19 +7912,19 @@
         <v>127</v>
       </c>
       <c r="C265" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D265" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="E265" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="F265" t="s">
-        <v>182</v>
-      </c>
-      <c r="G265" s="2" t="s">
-        <v>201</v>
+        <v>163</v>
+      </c>
+      <c r="G265" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.3">
@@ -7929,16 +7935,16 @@
         <v>127</v>
       </c>
       <c r="C266" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D266" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E266" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="F266" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="G266" s="2" t="s">
         <v>201</v>
@@ -7952,16 +7958,16 @@
         <v>127</v>
       </c>
       <c r="C267" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D267" t="s">
-        <v>149</v>
+        <v>236</v>
       </c>
       <c r="E267" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F267" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G267" s="2" t="s">
         <v>201</v>
@@ -7975,16 +7981,16 @@
         <v>127</v>
       </c>
       <c r="C268" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D268" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="E268" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F268" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G268" s="2" t="s">
         <v>201</v>
@@ -7998,19 +8004,19 @@
         <v>127</v>
       </c>
       <c r="C269" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D269" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="E269" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F269" t="s">
-        <v>182</v>
-      </c>
-      <c r="G269" s="2" t="s">
-        <v>201</v>
+        <v>180</v>
+      </c>
+      <c r="G269" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.3">
@@ -8024,16 +8030,16 @@
         <v>8</v>
       </c>
       <c r="D270" t="s">
-        <v>49</v>
+        <v>239</v>
       </c>
       <c r="E270" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F270" t="s">
-        <v>183</v>
-      </c>
-      <c r="G270" s="2" t="s">
-        <v>201</v>
+        <v>180</v>
+      </c>
+      <c r="G270" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.3">
@@ -8044,19 +8050,19 @@
         <v>127</v>
       </c>
       <c r="C271" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D271" t="s">
-        <v>241</v>
+        <v>153</v>
       </c>
       <c r="E271" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F271" t="s">
-        <v>183</v>
-      </c>
-      <c r="G271" s="2" t="s">
-        <v>201</v>
+        <v>181</v>
+      </c>
+      <c r="G271" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.3">
@@ -8070,13 +8076,13 @@
         <v>8</v>
       </c>
       <c r="D272" t="s">
-        <v>242</v>
+        <v>154</v>
       </c>
       <c r="E272" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F272" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G272" s="2" t="s">
         <v>201</v>
@@ -8093,13 +8099,13 @@
         <v>8</v>
       </c>
       <c r="D273" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E273" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F273" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G273" s="2" t="s">
         <v>201</v>
@@ -8107,22 +8113,22 @@
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>155</v>
+        <v>76</v>
       </c>
       <c r="B274" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="C274" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D274" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="E274" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="F274" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="G274" s="2" t="s">
         <v>201</v>
@@ -8130,45 +8136,45 @@
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>155</v>
+        <v>76</v>
       </c>
       <c r="B275" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="C275" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D275" t="s">
-        <v>52</v>
+        <v>134</v>
       </c>
       <c r="E275" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F275" t="s">
-        <v>185</v>
-      </c>
-      <c r="G275" s="1" t="s">
-        <v>161</v>
+        <v>182</v>
+      </c>
+      <c r="G275" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>155</v>
+        <v>76</v>
       </c>
       <c r="B276" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="C276" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D276" t="s">
-        <v>52</v>
+        <v>153</v>
       </c>
       <c r="E276" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F276" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G276" s="2" t="s">
         <v>201</v>
@@ -8176,139 +8182,369 @@
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>155</v>
+        <v>76</v>
       </c>
       <c r="B277" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="C277" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D277" t="s">
-        <v>54</v>
+        <v>149</v>
       </c>
       <c r="E277" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F277" t="s">
-        <v>187</v>
-      </c>
-      <c r="G277" t="s">
-        <v>161</v>
+        <v>182</v>
+      </c>
+      <c r="G277" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>155</v>
+        <v>76</v>
       </c>
       <c r="B278" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="C278" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D278" t="s">
-        <v>39</v>
+        <v>233</v>
       </c>
       <c r="E278" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F278" t="s">
-        <v>176</v>
-      </c>
-      <c r="G278" t="s">
-        <v>161</v>
+        <v>182</v>
+      </c>
+      <c r="G278" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>155</v>
+        <v>76</v>
       </c>
       <c r="B279" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="C279" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D279" t="s">
-        <v>24</v>
+        <v>235</v>
       </c>
       <c r="E279" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="F279" t="s">
-        <v>168</v>
-      </c>
-      <c r="G279" s="1" t="s">
-        <v>161</v>
+        <v>182</v>
+      </c>
+      <c r="G279" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>155</v>
+        <v>76</v>
       </c>
       <c r="B280" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="C280" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D280" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="E280" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="F280" t="s">
-        <v>172</v>
-      </c>
-      <c r="G280" s="1" t="s">
-        <v>161</v>
+        <v>183</v>
+      </c>
+      <c r="G280" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>155</v>
+        <v>76</v>
       </c>
       <c r="B281" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="C281" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D281" t="s">
-        <v>33</v>
+        <v>241</v>
       </c>
       <c r="E281" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="F281" t="s">
-        <v>172</v>
-      </c>
-      <c r="G281" s="1" t="s">
-        <v>161</v>
+        <v>183</v>
+      </c>
+      <c r="G281" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
+        <v>76</v>
+      </c>
+      <c r="B282" t="s">
+        <v>127</v>
+      </c>
+      <c r="C282" t="s">
+        <v>8</v>
+      </c>
+      <c r="D282" t="s">
+        <v>242</v>
+      </c>
+      <c r="E282" t="s">
+        <v>49</v>
+      </c>
+      <c r="F282" t="s">
+        <v>183</v>
+      </c>
+      <c r="G282" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A283" t="s">
+        <v>76</v>
+      </c>
+      <c r="B283" t="s">
+        <v>127</v>
+      </c>
+      <c r="C283" t="s">
+        <v>8</v>
+      </c>
+      <c r="D283" t="s">
+        <v>239</v>
+      </c>
+      <c r="E283" t="s">
+        <v>49</v>
+      </c>
+      <c r="F283" t="s">
+        <v>183</v>
+      </c>
+      <c r="G283" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A284" t="s">
         <v>155</v>
       </c>
-      <c r="B282" t="s">
+      <c r="B284" t="s">
+        <v>156</v>
+      </c>
+      <c r="C284" t="s">
+        <v>23</v>
+      </c>
+      <c r="D284" t="s">
+        <v>157</v>
+      </c>
+      <c r="E284" t="s">
+        <v>35</v>
+      </c>
+      <c r="F284" t="s">
+        <v>174</v>
+      </c>
+      <c r="G284" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A285" t="s">
+        <v>155</v>
+      </c>
+      <c r="B285" t="s">
+        <v>158</v>
+      </c>
+      <c r="C285" t="s">
+        <v>23</v>
+      </c>
+      <c r="D285" t="s">
+        <v>52</v>
+      </c>
+      <c r="E285" t="s">
+        <v>52</v>
+      </c>
+      <c r="F285" t="s">
+        <v>185</v>
+      </c>
+      <c r="G285" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A286" t="s">
+        <v>155</v>
+      </c>
+      <c r="B286" t="s">
+        <v>158</v>
+      </c>
+      <c r="C286" t="s">
+        <v>18</v>
+      </c>
+      <c r="D286" t="s">
+        <v>52</v>
+      </c>
+      <c r="E286" t="s">
+        <v>52</v>
+      </c>
+      <c r="F286" t="s">
+        <v>185</v>
+      </c>
+      <c r="G286" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A287" t="s">
+        <v>155</v>
+      </c>
+      <c r="B287" t="s">
+        <v>158</v>
+      </c>
+      <c r="C287" t="s">
+        <v>23</v>
+      </c>
+      <c r="D287" t="s">
+        <v>54</v>
+      </c>
+      <c r="E287" t="s">
+        <v>54</v>
+      </c>
+      <c r="F287" t="s">
+        <v>187</v>
+      </c>
+      <c r="G287" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A288" t="s">
+        <v>155</v>
+      </c>
+      <c r="B288" t="s">
+        <v>158</v>
+      </c>
+      <c r="C288" t="s">
+        <v>10</v>
+      </c>
+      <c r="D288" t="s">
+        <v>39</v>
+      </c>
+      <c r="E288" t="s">
+        <v>39</v>
+      </c>
+      <c r="F288" t="s">
+        <v>176</v>
+      </c>
+      <c r="G288" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A289" t="s">
+        <v>155</v>
+      </c>
+      <c r="B289" t="s">
         <v>159</v>
       </c>
-      <c r="C282" t="s">
+      <c r="C289" t="s">
+        <v>10</v>
+      </c>
+      <c r="D289" t="s">
+        <v>24</v>
+      </c>
+      <c r="E289" t="s">
+        <v>24</v>
+      </c>
+      <c r="F289" t="s">
+        <v>168</v>
+      </c>
+      <c r="G289" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A290" t="s">
+        <v>155</v>
+      </c>
+      <c r="B290" t="s">
+        <v>159</v>
+      </c>
+      <c r="C290" t="s">
+        <v>23</v>
+      </c>
+      <c r="D290" t="s">
+        <v>33</v>
+      </c>
+      <c r="E290" t="s">
+        <v>33</v>
+      </c>
+      <c r="F290" t="s">
+        <v>172</v>
+      </c>
+      <c r="G290" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A291" t="s">
+        <v>155</v>
+      </c>
+      <c r="B291" t="s">
+        <v>159</v>
+      </c>
+      <c r="C291" t="s">
+        <v>10</v>
+      </c>
+      <c r="D291" t="s">
+        <v>33</v>
+      </c>
+      <c r="E291" t="s">
+        <v>33</v>
+      </c>
+      <c r="F291" t="s">
+        <v>172</v>
+      </c>
+      <c r="G291" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A292" t="s">
+        <v>155</v>
+      </c>
+      <c r="B292" t="s">
+        <v>159</v>
+      </c>
+      <c r="C292" t="s">
         <v>21</v>
       </c>
-      <c r="D282" t="s">
+      <c r="D292" t="s">
         <v>160</v>
       </c>
-      <c r="E282" t="s">
+      <c r="E292" t="s">
         <v>39</v>
       </c>
-      <c r="F282" t="s">
+      <c r="F292" t="s">
         <v>176</v>
       </c>
-      <c r="G282" s="2" t="s">
+      <c r="G292" s="2" t="s">
         <v>201</v>
       </c>
     </row>

</xml_diff>